<commit_message>
updated current week show mode
</commit_message>
<xml_diff>
--- a/class.xlsx
+++ b/class.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Royal\PycharmProjects\classCalendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3496E1E3-6C51-4F08-BF0F-46F741A51B45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CEC82E-A165-4790-8FDA-C0580E35B3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>电子信息与电气工程学部</t>
   </si>
@@ -48,124 +48,130 @@
     <t>否</t>
   </si>
   <si>
-    <t>电网络理论1</t>
-  </si>
-  <si>
-    <t>研教楼508</t>
-  </si>
-  <si>
-    <t>电网络理论</t>
-  </si>
-  <si>
-    <t>周玮</t>
-  </si>
-  <si>
-    <t>6-17周 单双周:星期一 上午1,2 星期四 上午1,2</t>
-  </si>
-  <si>
-    <t>现代控制工程1</t>
-  </si>
-  <si>
-    <t>研教楼412</t>
-  </si>
-  <si>
-    <t>现代控制工程</t>
-  </si>
-  <si>
-    <t>王东</t>
-  </si>
-  <si>
-    <t>2-13周 单双周:星期二 下午5,6 星期四 下午5,6</t>
-  </si>
-  <si>
-    <t>论文写作与学术规范5</t>
-  </si>
-  <si>
-    <t>论文写作与学术规范</t>
-  </si>
-  <si>
-    <t>胡志刚</t>
-  </si>
-  <si>
-    <t>6-9周 单双周:星期五 下午5,6,7,8</t>
-  </si>
-  <si>
-    <t>中国特色社会主义理论与实践研究12</t>
-  </si>
-  <si>
-    <t>研教楼203</t>
-  </si>
-  <si>
-    <t>马克思主义学院</t>
-  </si>
-  <si>
-    <t>中国特色社会主义理论与实践研究</t>
-  </si>
-  <si>
-    <t>魏晓文</t>
-  </si>
-  <si>
-    <t>9-17周 单双周:星期五 上午1,2,3,4</t>
-  </si>
-  <si>
-    <t>口语交流 II （学术交流）8</t>
-  </si>
-  <si>
-    <t>口语交流 II （学术交流）</t>
-  </si>
-  <si>
-    <t>时真妹</t>
-  </si>
-  <si>
-    <t>2-17周 双周:星期三 上午3,4</t>
-  </si>
-  <si>
-    <t>矩阵与数值分析3</t>
-  </si>
-  <si>
-    <t>研教楼204</t>
-  </si>
-  <si>
-    <t>数学科学学院</t>
-  </si>
-  <si>
-    <t>矩阵与数值分析</t>
-  </si>
-  <si>
-    <t>金光日</t>
-  </si>
-  <si>
-    <t>2-14周 单双周:星期一 下午5,6 星期三 下午5,6</t>
-  </si>
-  <si>
-    <t>电力系统无功电压控制1</t>
-  </si>
-  <si>
-    <t>研教楼202</t>
-  </si>
-  <si>
-    <t>电力系统无功电压控制</t>
-  </si>
-  <si>
-    <t>孙辉</t>
-  </si>
-  <si>
-    <t>2-7周 单双周:星期二 上午3,4 星期五 上午3,4 星期日 下午7,8</t>
-  </si>
-  <si>
-    <t>深度学习与算法设计2</t>
-  </si>
-  <si>
-    <t>研教楼304</t>
-  </si>
-  <si>
-    <t>深度学习与算法设计</t>
-  </si>
-  <si>
-    <t>王一帆</t>
-  </si>
-  <si>
-    <t>10-17周 单双周:星期二 上午3,4 星期四 上午3,4</t>
+    <t>高电压工程1</t>
+  </si>
+  <si>
+    <t>研教楼414</t>
+  </si>
+  <si>
+    <t>高电压工程</t>
+  </si>
+  <si>
+    <t>段雄英</t>
+  </si>
+  <si>
+    <t>2-9周 单双周:星期一 上午3,4 星期四 上午3,4</t>
+  </si>
+  <si>
+    <t>电气工程基础及应用（双语授课）1</t>
+  </si>
+  <si>
+    <t>研教楼306</t>
+  </si>
+  <si>
+    <t>电气工程基础及应用（双语授课）</t>
+  </si>
+  <si>
+    <t>刘蕴红</t>
+  </si>
+  <si>
+    <t>10-17周 单双周:星期二 上午1,2 星期五 上午1,2</t>
+  </si>
+  <si>
+    <t>工程伦理1</t>
+  </si>
+  <si>
+    <t>研教楼102</t>
+  </si>
+  <si>
+    <t>工程伦理</t>
+  </si>
+  <si>
+    <t>魏东兴</t>
+  </si>
+  <si>
+    <t>10-13周 单双周:星期二 下午5,6,7,8</t>
+  </si>
+  <si>
+    <t>知识产权6</t>
+  </si>
+  <si>
+    <t>知识产权</t>
+  </si>
+  <si>
+    <t>郭玉坤</t>
+  </si>
+  <si>
+    <t>10-13周 单双周:星期三 上午1,2,3,4</t>
+  </si>
+  <si>
+    <t>信息检索5</t>
+  </si>
+  <si>
+    <t>信息检索</t>
+  </si>
+  <si>
+    <t>叶颖涵</t>
+  </si>
+  <si>
+    <t>10-13周 单双周:星期三 下午5,6,7,8</t>
+  </si>
+  <si>
+    <t>阅读与写作 I （基础读写技能）40</t>
+  </si>
+  <si>
+    <t>阅读与写作 I （基础读写技能）</t>
+  </si>
+  <si>
+    <t>程哲</t>
+  </si>
+  <si>
+    <t>3-18周 单周:星期五 下午7,8</t>
+  </si>
+  <si>
+    <t>电力开关技术与应用1</t>
+  </si>
+  <si>
+    <t>研教楼210</t>
+  </si>
+  <si>
+    <t>电力开关技术与应用</t>
+  </si>
+  <si>
+    <t>董恩源</t>
+  </si>
+  <si>
+    <t>2-9周 单双周:星期五 上午3,4</t>
+  </si>
+  <si>
+    <t>研教楼507</t>
+  </si>
+  <si>
+    <t>2-9周 单双周:星期二 上午3,4</t>
+  </si>
+  <si>
+    <t>环境电工技术1</t>
+  </si>
+  <si>
+    <t>环境电工技术</t>
+  </si>
+  <si>
+    <t>姜楠</t>
+  </si>
+  <si>
+    <t>2-9周 单双周:星期三 下午5,6 星期四 下午5,6</t>
+  </si>
+  <si>
+    <t>气体放电物理1</t>
+  </si>
+  <si>
+    <t>气体放电物理</t>
+  </si>
+  <si>
+    <t>鲁娜</t>
+  </si>
+  <si>
+    <t>2-9周 单双周:星期一 下午5,6 星期五 晚上9,10</t>
   </si>
 </sst>
 </file>
@@ -490,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
@@ -512,7 +518,7 @@
         <v>0</v>
       </c>
       <c r="D1">
-        <v>2020130023</v>
+        <v>2020130013</v>
       </c>
       <c r="E1" t="s">
         <v>9</v>
@@ -524,10 +530,10 @@
         <v>11</v>
       </c>
       <c r="H1">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="I1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -544,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>2020520023</v>
+        <v>2020140153</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -556,10 +562,10 @@
         <v>16</v>
       </c>
       <c r="H2">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" t="s">
         <v>1</v>
@@ -570,22 +576,22 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3">
-        <v>2070110059</v>
+        <v>2070110041</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -599,31 +605,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2070110062</v>
+      </c>
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="D4">
-        <v>2070310013</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
       <c r="H4">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" t="s">
         <v>1</v>
@@ -631,25 +637,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2070110072</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>2100010021</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
       </c>
       <c r="H5">
         <v>16</v>
@@ -663,31 +669,31 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>2100010033</v>
+      </c>
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>33</v>
       </c>
-      <c r="D6">
-        <v>2120020013</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
       <c r="H6">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" t="s">
         <v>1</v>
@@ -695,25 +701,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>2020140143</v>
+        <v>2020140023</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H7">
         <v>32</v>
@@ -727,25 +733,25 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>2020420013</v>
+        <v>2020140023</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H8">
         <v>32</v>
@@ -754,6 +760,70 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2020140083</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9">
+        <v>32</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>2020140103</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10">
+        <v>32</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>